<commit_message>
Modified 004 footer test case
</commit_message>
<xml_diff>
--- a/Resources/TestData/qat02.xlsx
+++ b/Resources/TestData/qat02.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="6540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="6540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REG" sheetId="4" r:id="rId1"/>
@@ -182,9 +182,6 @@
     <t>http://investor.frontier.com/releases.cfm</t>
   </si>
   <si>
-    <t>https://frontier.com/corporate/pressroom</t>
-  </si>
-  <si>
     <t>Public_Inspection_Files_Url</t>
   </si>
   <si>
@@ -753,6 +750,9 @@
   </si>
   <si>
     <t>12/04/17 - 1/03/18</t>
+  </si>
+  <si>
+    <t>https://frontier.com/corporate/news/home</t>
   </si>
 </sst>
 </file>
@@ -1261,7 +1261,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1307,7 +1307,7 @@
         <v>27</v>
       </c>
       <c r="E1" s="34" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F1" s="34" t="s">
         <v>20</v>
@@ -1316,43 +1316,43 @@
         <v>21</v>
       </c>
       <c r="H1" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="I1" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="J1" s="34" t="s">
         <v>149</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="K1" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="L1" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="M1" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="L1" s="34" t="s">
-        <v>151</v>
-      </c>
-      <c r="M1" s="34" t="s">
+      <c r="N1" s="35" t="s">
         <v>153</v>
       </c>
-      <c r="N1" s="35" t="s">
-        <v>154</v>
-      </c>
       <c r="O1" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="P1" s="35" t="s">
         <v>158</v>
       </c>
-      <c r="P1" s="35" t="s">
+      <c r="Q1" s="35" t="s">
         <v>159</v>
       </c>
-      <c r="Q1" s="35" t="s">
-        <v>160</v>
-      </c>
       <c r="R1" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="S1" s="35" t="s">
         <v>236</v>
       </c>
-      <c r="S1" s="35" t="s">
+      <c r="T1" s="10" t="s">
         <v>237</v>
-      </c>
-      <c r="T1" s="10" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -1360,22 +1360,22 @@
         <v>2</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C2" s="35" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E2" s="35" t="s">
         <v>19</v>
       </c>
       <c r="F2" s="36" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H2" s="35"/>
       <c r="I2" s="35"/>
@@ -1396,40 +1396,40 @@
         <v>3</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C3" s="35" t="s">
         <v>18</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E3" s="35" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="36" t="s">
+        <v>208</v>
+      </c>
+      <c r="G3" s="35" t="s">
+        <v>128</v>
+      </c>
+      <c r="H3" s="35" t="s">
         <v>209</v>
       </c>
-      <c r="G3" s="35" t="s">
-        <v>129</v>
-      </c>
-      <c r="H3" s="35" t="s">
+      <c r="I3" s="35" t="s">
+        <v>238</v>
+      </c>
+      <c r="J3" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="K3" s="35" t="s">
         <v>210</v>
       </c>
-      <c r="I3" s="35" t="s">
+      <c r="L3" s="35" t="s">
         <v>239</v>
       </c>
-      <c r="J3" s="35" t="s">
-        <v>241</v>
-      </c>
-      <c r="K3" s="35" t="s">
+      <c r="M3" s="35" t="s">
         <v>211</v>
-      </c>
-      <c r="L3" s="35" t="s">
-        <v>240</v>
-      </c>
-      <c r="M3" s="35" t="s">
-        <v>212</v>
       </c>
       <c r="N3" s="35"/>
       <c r="O3" s="35"/>
@@ -1444,22 +1444,22 @@
         <v>4</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C4" s="35" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E4" s="35" t="s">
         <v>19</v>
       </c>
       <c r="F4" s="36" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G4" s="35" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H4" s="35"/>
       <c r="I4" s="35"/>
@@ -1468,16 +1468,16 @@
       <c r="L4" s="35"/>
       <c r="M4" s="35"/>
       <c r="N4" s="35" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O4" s="35" t="s">
+        <v>160</v>
+      </c>
+      <c r="P4" s="35" t="s">
         <v>161</v>
       </c>
-      <c r="P4" s="35" t="s">
-        <v>162</v>
-      </c>
       <c r="Q4" s="35" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="R4" s="35"/>
       <c r="S4" s="35"/>
@@ -1488,22 +1488,22 @@
         <v>5</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C5" s="35" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E5" s="35" t="s">
         <v>19</v>
       </c>
       <c r="F5" s="36" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G5" s="35" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H5" s="35"/>
       <c r="I5" s="35"/>
@@ -1524,22 +1524,22 @@
         <v>6</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C6" s="35" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E6" s="35" t="s">
         <v>19</v>
       </c>
       <c r="F6" s="36" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G6" s="35" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H6" s="35"/>
       <c r="I6" s="35"/>
@@ -1552,10 +1552,10 @@
       <c r="P6" s="35"/>
       <c r="Q6" s="35"/>
       <c r="R6" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="S6" s="35" t="s">
         <v>207</v>
-      </c>
-      <c r="S6" s="35" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -1563,22 +1563,22 @@
         <v>7</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C7" s="35" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E7" s="35" t="s">
         <v>19</v>
       </c>
       <c r="F7" s="36" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G7" s="35" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H7" s="35"/>
       <c r="I7" s="35"/>
@@ -1593,7 +1593,7 @@
       <c r="R7" s="35"/>
       <c r="S7" s="35"/>
       <c r="T7" s="35" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -1601,22 +1601,22 @@
         <v>10</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C8" s="35" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E8" s="35" t="s">
         <v>19</v>
       </c>
       <c r="F8" s="36" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G8" s="35" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H8" s="35"/>
       <c r="I8" s="35"/>
@@ -1637,22 +1637,22 @@
         <v>11</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C9" s="35" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="36" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E9" s="35" t="s">
         <v>19</v>
       </c>
       <c r="F9" s="36" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G9" s="35" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H9" s="35"/>
       <c r="I9" s="35"/>
@@ -1683,11 +1683,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BM17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="AF2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BQ17" sqref="BQ17"/>
+      <selection pane="bottomRight" activeCell="AF5" sqref="AF5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1771,13 +1771,13 @@
         <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>28</v>
@@ -1813,7 +1813,7 @@
         <v>39</v>
       </c>
       <c r="R1" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="S1" s="10" t="s">
         <v>40</v>
@@ -1840,121 +1840,121 @@
         <v>42</v>
       </c>
       <c r="AA1" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AB1" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AC1" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AD1" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AE1" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AF1" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AG1" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="AH1" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI1" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="AJ1" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK1" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="AH1" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI1" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="AJ1" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="AK1" s="13" t="s">
+      <c r="AL1" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM1" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="AN1" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO1" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="AP1" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="AQ1" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="AL1" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="AM1" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="AN1" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="AO1" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="AP1" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="AQ1" s="13" t="s">
+      <c r="AR1" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="AR1" s="14" t="s">
+      <c r="AS1" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="AS1" s="14" t="s">
+      <c r="AT1" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="AT1" s="14" t="s">
+      <c r="AU1" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="AU1" s="14" t="s">
+      <c r="AV1" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="AV1" s="14" t="s">
+      <c r="AW1" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="AW1" s="14" t="s">
+      <c r="AX1" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="AX1" s="14" t="s">
+      <c r="AY1" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="AY1" s="14" t="s">
-        <v>173</v>
-      </c>
       <c r="AZ1" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="BA1" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="BB1" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="BC1" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="BC1" s="10" t="s">
+      <c r="BD1" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="BD1" s="7" t="s">
-        <v>93</v>
-      </c>
       <c r="BE1" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="BF1" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="BG1" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="BH1" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="BI1" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BJ1" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="BK1" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="BL1" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="BM1" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:65" x14ac:dyDescent="0.25">
@@ -1968,34 +1968,34 @@
         <v>18</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="L2" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>186</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>187</v>
       </c>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
@@ -2055,10 +2055,10 @@
         <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>19</v>
@@ -2071,22 +2071,22 @@
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="O3" s="5" t="s">
         <v>36</v>
       </c>
       <c r="P3" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q3" s="19" t="s">
         <v>188</v>
-      </c>
-      <c r="Q3" s="19" t="s">
-        <v>189</v>
       </c>
       <c r="R3" s="19" t="s">
         <v>41</v>
       </c>
       <c r="S3" s="19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
@@ -2146,10 +2146,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>19</v>
@@ -2168,25 +2168,25 @@
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
       <c r="T4" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="V4" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="U4" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="V4" s="4" t="s">
+      <c r="W4" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="W4" s="4" t="s">
+      <c r="X4" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="X4" s="4" t="s">
+      <c r="Y4" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="Y4" s="4" t="s">
+      <c r="Z4" s="4" t="s">
         <v>194</v>
-      </c>
-      <c r="Z4" s="4" t="s">
-        <v>195</v>
       </c>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
@@ -2239,10 +2239,10 @@
         <v>18</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>19</v>
@@ -2268,7 +2268,7 @@
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
       <c r="AA5" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AB5" s="4" t="s">
         <v>49</v>
@@ -2277,19 +2277,19 @@
         <v>50</v>
       </c>
       <c r="AD5" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="AE5" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="AE5" s="4" t="s">
+      <c r="AF5" s="36" t="s">
+        <v>241</v>
+      </c>
+      <c r="AG5" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="AF5" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AG5" s="4" t="s">
+      <c r="AH5" s="4" t="s">
         <v>199</v>
-      </c>
-      <c r="AH5" s="4" t="s">
-        <v>200</v>
       </c>
       <c r="AI5" s="2"/>
       <c r="AJ5" s="2"/>
@@ -2328,16 +2328,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>19</v>
@@ -2371,31 +2371,31 @@
       <c r="AG6" s="2"/>
       <c r="AH6" s="2"/>
       <c r="AI6" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="AJ6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK6" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN6" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AO6" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AP6" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AQ6" s="4" t="s">
         <v>156</v>
-      </c>
-      <c r="AJ6" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="AK6" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="AL6" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM6" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="AN6" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="AO6" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AP6" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AQ6" s="4" t="s">
-        <v>157</v>
       </c>
       <c r="AR6" s="2"/>
       <c r="AS6" s="2"/>
@@ -2425,16 +2425,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>19</v>
@@ -2477,28 +2477,28 @@
       <c r="AP7" s="2"/>
       <c r="AQ7" s="2"/>
       <c r="AR7" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AS7" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="AS7" s="17" t="s">
+      <c r="AT7" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="AU7" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="AT7" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="AU7" s="4" t="s">
+      <c r="AV7" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="AV7" s="4" t="s">
+      <c r="AW7" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="AW7" s="17" t="s">
-        <v>78</v>
-      </c>
       <c r="AX7" s="17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AY7" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AZ7" s="2"/>
       <c r="BA7" s="2"/>
@@ -2520,16 +2520,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>19</v>
@@ -2580,7 +2580,7 @@
       <c r="AX8" s="2"/>
       <c r="AY8" s="2"/>
       <c r="AZ8" s="17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="BA8" s="2"/>
       <c r="BB8" s="2"/>
@@ -2601,16 +2601,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>19</v>
@@ -2662,7 +2662,7 @@
       <c r="AY9" s="2"/>
       <c r="AZ9" s="2"/>
       <c r="BA9" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="BB9" s="2"/>
       <c r="BC9" s="2"/>
@@ -2682,16 +2682,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>19</v>
@@ -2744,7 +2744,7 @@
       <c r="AZ10" s="2"/>
       <c r="BA10" s="2"/>
       <c r="BB10" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="BC10" s="2"/>
       <c r="BD10" s="2"/>
@@ -2763,16 +2763,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>19</v>
@@ -2826,7 +2826,7 @@
       <c r="BA11" s="2"/>
       <c r="BB11" s="2"/>
       <c r="BC11" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="BD11" s="2"/>
       <c r="BE11" s="2"/>
@@ -2844,16 +2844,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>19</v>
@@ -2908,7 +2908,7 @@
       <c r="BB12" s="2"/>
       <c r="BC12" s="2"/>
       <c r="BD12" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="BE12" s="2"/>
       <c r="BF12" s="2"/>
@@ -2925,16 +2925,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>19</v>
@@ -2990,10 +2990,10 @@
       <c r="BC13" s="2"/>
       <c r="BD13" s="2"/>
       <c r="BE13" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="BF13" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="BF13" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="BG13" s="2"/>
       <c r="BH13" s="2"/>
@@ -3008,16 +3008,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>19</v>
@@ -3075,7 +3075,7 @@
       <c r="BE14" s="2"/>
       <c r="BF14" s="2"/>
       <c r="BG14" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BH14" s="2"/>
       <c r="BI14" s="2"/>
@@ -3089,16 +3089,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>19</v>
@@ -3157,10 +3157,10 @@
       <c r="BF15" s="2"/>
       <c r="BG15" s="2"/>
       <c r="BH15" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="BI15" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="BI15" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="BJ15" s="2"/>
       <c r="BK15" s="2"/>
@@ -3172,16 +3172,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>19</v>
@@ -3242,10 +3242,10 @@
       <c r="BH16" s="2"/>
       <c r="BI16" s="2"/>
       <c r="BJ16" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="BK16" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="BK16" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="BL16" s="2"/>
       <c r="BM16" s="2"/>
@@ -3255,16 +3255,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>19</v>
@@ -3327,10 +3327,10 @@
       <c r="BJ17" s="2"/>
       <c r="BK17" s="2"/>
       <c r="BL17" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="BM17" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="BM17" s="2" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -3435,13 +3435,13 @@
         <v>17</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E1" s="20" t="s">
         <v>27</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G1" s="20" t="s">
         <v>20</v>
@@ -3450,16 +3450,16 @@
         <v>21</v>
       </c>
       <c r="I1" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="J1" s="27" t="s">
+        <v>132</v>
+      </c>
+      <c r="K1" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="J1" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="K1" s="27" t="s">
+      <c r="L1" s="27" t="s">
         <v>131</v>
-      </c>
-      <c r="L1" s="27" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -3467,16 +3467,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C2" s="22" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E2" s="36" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F2" s="22" t="s">
         <v>19</v>
@@ -3484,16 +3484,16 @@
       <c r="G2" s="25"/>
       <c r="H2" s="23"/>
       <c r="I2" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="J2" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="K2" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="L2" s="24" t="s">
         <v>125</v>
-      </c>
-      <c r="J2" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="K2" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="L2" s="24" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -3501,16 +3501,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C3" s="22" t="s">
         <v>18</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F3" s="22" t="s">
         <v>19</v>
@@ -3527,25 +3527,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F4" s="22" t="s">
         <v>19</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H4" s="22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I4" s="22"/>
       <c r="J4" s="22"/>
@@ -3557,16 +3557,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C5" s="22" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F5" s="22" t="s">
         <v>19</v>
@@ -3583,16 +3583,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C6" s="22" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F6" s="22" t="s">
         <v>19</v>
@@ -3609,16 +3609,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C7" s="22" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F7" s="22" t="s">
         <v>19</v>
@@ -3635,16 +3635,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C8" s="22" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F8" s="22" t="s">
         <v>19</v>
@@ -3661,16 +3661,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C9" s="22" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F9" s="22" t="s">
         <v>19</v>
@@ -3687,16 +3687,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C10" s="22" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F10" s="22" t="s">
         <v>19</v>
@@ -3766,52 +3766,52 @@
         <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G1" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="H1" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="I1" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="J1" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="K1" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="K1" s="33" t="s">
+      <c r="L1" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="L1" s="33" t="s">
-        <v>140</v>
-      </c>
       <c r="M1" s="33" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="N1" s="33" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O1" s="33" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="P1" s="33" t="s">
         <v>46</v>
       </c>
       <c r="Q1" s="33" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="R1" s="33" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="S1" s="33" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -3819,22 +3819,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C2" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="28" t="s">
+        <v>179</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="29" t="s">
         <v>180</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>178</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>181</v>
       </c>
       <c r="H2" s="29"/>
       <c r="I2" s="29"/>
@@ -3848,23 +3848,23 @@
         <v>2</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C3" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F3" s="28" t="s">
         <v>19</v>
       </c>
       <c r="G3" s="28"/>
       <c r="H3" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I3" s="28"/>
       <c r="J3" s="28"/>
@@ -3883,16 +3883,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C4" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F4" s="28" t="s">
         <v>19</v>
@@ -3900,7 +3900,7 @@
       <c r="G4" s="28"/>
       <c r="H4" s="28"/>
       <c r="I4" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J4" s="28"/>
       <c r="K4" s="28"/>
@@ -3918,16 +3918,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C5" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F5" s="28" t="s">
         <v>19</v>
@@ -3936,7 +3936,7 @@
       <c r="H5" s="28"/>
       <c r="I5" s="28"/>
       <c r="J5" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K5" s="28"/>
       <c r="L5" s="28"/>
@@ -3953,16 +3953,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C6" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F6" s="28" t="s">
         <v>19</v>
@@ -3972,7 +3972,7 @@
       <c r="I6" s="28"/>
       <c r="J6" s="28"/>
       <c r="K6" s="36" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L6" s="28"/>
       <c r="M6" s="28"/>
@@ -3988,16 +3988,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C7" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F7" s="28" t="s">
         <v>19</v>
@@ -4008,7 +4008,7 @@
       <c r="J7" s="28"/>
       <c r="K7" s="28"/>
       <c r="L7" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="M7" s="28"/>
       <c r="N7" s="28"/>
@@ -4023,16 +4023,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C8" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F8" s="28" t="s">
         <v>19</v>
@@ -4056,16 +4056,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C9" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F9" s="28" t="s">
         <v>19</v>
@@ -4089,16 +4089,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C10" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F10" s="28" t="s">
         <v>19</v>
@@ -4122,16 +4122,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="35" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C11" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F11" s="28" t="s">
         <v>19</v>
@@ -4143,7 +4143,7 @@
       <c r="K11" s="28"/>
       <c r="L11" s="28"/>
       <c r="M11" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="N11" s="28"/>
       <c r="O11" s="28"/>
@@ -4157,16 +4157,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C12" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F12" s="28" t="s">
         <v>19</v>
@@ -4179,7 +4179,7 @@
       <c r="L12" s="28"/>
       <c r="M12" s="28"/>
       <c r="N12" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O12" s="28"/>
       <c r="P12" s="28"/>
@@ -4192,16 +4192,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C13" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E13" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F13" s="28" t="s">
         <v>19</v>
@@ -4215,7 +4215,7 @@
       <c r="M13" s="28"/>
       <c r="N13" s="28"/>
       <c r="O13" s="19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="P13" s="28"/>
       <c r="Q13" s="28"/>
@@ -4227,16 +4227,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C14" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F14" s="28" t="s">
         <v>19</v>
@@ -4251,7 +4251,7 @@
       <c r="N14" s="28"/>
       <c r="O14" s="28"/>
       <c r="P14" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="Q14" s="28"/>
       <c r="R14" s="28"/>
@@ -4262,16 +4262,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C15" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E15" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F15" s="28" t="s">
         <v>19</v>
@@ -4287,7 +4287,7 @@
       <c r="O15" s="28"/>
       <c r="P15" s="28"/>
       <c r="Q15" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="R15" s="28"/>
       <c r="S15" s="28"/>
@@ -4297,16 +4297,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C16" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F16" s="28" t="s">
         <v>19</v>
@@ -4323,7 +4323,7 @@
       <c r="P16" s="28"/>
       <c r="Q16" s="28"/>
       <c r="R16" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="S16" s="28"/>
     </row>
@@ -4332,16 +4332,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C17" s="28" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E17" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F17" s="28" t="s">
         <v>19</v>
@@ -4359,7 +4359,7 @@
       <c r="Q17" s="28"/>
       <c r="R17" s="28"/>
       <c r="S17" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ecom test cases added
</commit_message>
<xml_diff>
--- a/Resources/TestData/qat02.xlsx
+++ b/Resources/TestData/qat02.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="127">
   <si>
     <t>TC_NO</t>
   </si>
@@ -364,6 +364,45 @@
   </si>
   <si>
     <t>ftrfrank1+feb18@gmail.com</t>
+  </si>
+  <si>
+    <t>TC17</t>
+  </si>
+  <si>
+    <t>TC18</t>
+  </si>
+  <si>
+    <t>TC19</t>
+  </si>
+  <si>
+    <t>TC20</t>
+  </si>
+  <si>
+    <t>TC21</t>
+  </si>
+  <si>
+    <t>TC22</t>
+  </si>
+  <si>
+    <t>TC23</t>
+  </si>
+  <si>
+    <t>TC24</t>
+  </si>
+  <si>
+    <t>TC25</t>
+  </si>
+  <si>
+    <t>002_CC_.COM_SS_AS_E-Com_AVP_Verify$6increase_CustomEssentialsPackage</t>
+  </si>
+  <si>
+    <t>003_CC_.COM_SS_AS_E-Com_AVP_Verify$6increase_CustomSportsPackage</t>
+  </si>
+  <si>
+    <t>004_CC_.COM_SS_AS_E-Com_AVP_Verify$6increase_ExtremePackage</t>
+  </si>
+  <si>
+    <t>005_CC_.COM_SS_AS_E-Com_AVP_Verify$6increase_UltimateVideoPackage</t>
   </si>
 </sst>
 </file>
@@ -509,7 +548,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -533,7 +572,8 @@
     <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -817,13 +857,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G24" sqref="G24"/>
+      <selection pane="bottomRight" activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1313,16 +1353,16 @@
       <c r="C14" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="21" t="s">
         <v>20</v>
       </c>
       <c r="E14" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="F14" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="G14" s="21" t="s">
+      <c r="G14" s="22" t="s">
         <v>23</v>
       </c>
       <c r="H14" s="13"/>
@@ -1335,6 +1375,327 @@
       <c r="O14" s="13"/>
       <c r="P14" s="13"/>
       <c r="Q14" s="13"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="G15" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="G16" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="G17" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="G18" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="13"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="13"/>
+      <c r="Q24" s="13"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="13"/>
+      <c r="Q25" s="13"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13"/>
+      <c r="P26" s="13"/>
+      <c r="Q26" s="13"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1348,9 +1709,17 @@
     <hyperlink ref="D12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="D14" r:id="rId9" xr:uid="{21BE66A9-6327-498E-8C2B-7FE2E11ADD59}"/>
     <hyperlink ref="F14" r:id="rId10" xr:uid="{12E2B49E-1545-4672-B4A6-DEB308365455}"/>
+    <hyperlink ref="D15" r:id="rId11" xr:uid="{9EBBF634-8706-4A3F-B35D-4E439A536F07}"/>
+    <hyperlink ref="F15" r:id="rId12" xr:uid="{1EAE3C99-A8B6-4606-9E0F-3F30F1A974E1}"/>
+    <hyperlink ref="D16" r:id="rId13" xr:uid="{3BF6D693-1A70-4082-AA38-B89E5A7E3D1E}"/>
+    <hyperlink ref="F16" r:id="rId14" xr:uid="{BB5D3DA6-CFF2-41F1-9364-ACCECDFA487D}"/>
+    <hyperlink ref="D17" r:id="rId15" xr:uid="{E5B91846-B0A7-4689-8939-6B633CD433E1}"/>
+    <hyperlink ref="F17" r:id="rId16" xr:uid="{27A838A4-C4AB-469F-92BD-B56F89856E93}"/>
+    <hyperlink ref="D18" r:id="rId17" xr:uid="{339F8C4E-F6A1-496F-8C6F-34444D3A3D27}"/>
+    <hyperlink ref="F18" r:id="rId18" xr:uid="{B47F81F5-8E63-4013-B98A-3DCC7EF34CE2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
 
@@ -1362,16 +1731,16 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1:E1048576"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" style="11" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" style="11" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" style="11" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="58.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" style="11" customWidth="1"/>
     <col min="6" max="7" width="6.7109375" style="11" customWidth="1"/>
     <col min="8" max="16384" width="6.7109375" style="11"/>
   </cols>
@@ -1403,7 +1772,7 @@
       <c r="C2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="19" t="s">
         <v>20</v>
       </c>
       <c r="E2" s="13" t="s">
@@ -1420,7 +1789,7 @@
       <c r="C3" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="19" t="s">
         <v>20</v>
       </c>
       <c r="E3" s="13" t="s">
@@ -1667,12 +2036,13 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="https://qat01.frontier.com/" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="D16" r:id="rId2" display="https://qat01.frontier.com/" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="D17" r:id="rId3" display="https://qat01.frontier.com/" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="D16" r:id="rId1" display="https://qat01.frontier.com/" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="D17" r:id="rId2" display="https://qat01.frontier.com/" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{2243F20E-836A-44C8-A7E8-FEF69ED0BABA}"/>
+    <hyperlink ref="D2" r:id="rId4" xr:uid="{4A26EF29-4866-422F-8BC1-B340F7348B64}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -1684,16 +2054,16 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1:E1048576"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="65.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" style="8" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" style="8" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" style="8" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" style="8" customWidth="1"/>
     <col min="6" max="6" width="31.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.28515625" style="8" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Fixed Link & Unlink
</commit_message>
<xml_diff>
--- a/Resources/TestData/qat02.xlsx
+++ b/Resources/TestData/qat02.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="126">
   <si>
     <t>TC_NO</t>
   </si>
@@ -135,12 +135,6 @@
     <t>006_CC_REG_RES_FCOM_Man_MyProfile-LinkAccount</t>
   </si>
   <si>
-    <t>81398647071107145</t>
-  </si>
-  <si>
-    <t>9191</t>
-  </si>
-  <si>
     <t>TC06</t>
   </si>
   <si>
@@ -168,12 +162,6 @@
     <t>016_CC_.COM_archive_REG_RES_FCOM_Man_ECOMM_InternetHOPUpgrade</t>
   </si>
   <si>
-    <t>Ftrfrank1+ecomauto@gmail.com</t>
-  </si>
-  <si>
-    <t>813-689-5758-092074-5 JOYCE T.</t>
-  </si>
-  <si>
     <t>TC10</t>
   </si>
   <si>
@@ -189,9 +177,6 @@
     <t>727-121-3162-021213-5 PATRICIA C.</t>
   </si>
   <si>
-    <t>Order #070480784</t>
-  </si>
-  <si>
     <t>TC11</t>
   </si>
   <si>
@@ -403,6 +388,18 @@
   </si>
   <si>
     <t>005_CC_.COM_SS_AS_E-Com_AVP_Verify$6increase_UltimateVideoPackage</t>
+  </si>
+  <si>
+    <t>21946240630331005</t>
+  </si>
+  <si>
+    <t>5050</t>
+  </si>
+  <si>
+    <t>Ftrfrank1+remedyticket@gmail.com</t>
+  </si>
+  <si>
+    <t>210-023-1679-051407-5 JOANN S.</t>
   </si>
 </sst>
 </file>
@@ -860,10 +857,10 @@
   <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L34" sqref="L34"/>
+      <selection pane="bottomRight" activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,7 +878,7 @@
     <col min="11" max="11" width="16.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24.85546875" style="11" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="31.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.7109375" style="11" customWidth="1"/>
     <col min="15" max="15" width="14.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="18.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16.7109375" style="11" bestFit="1" customWidth="1"/>
@@ -1102,8 +1099,8 @@
       <c r="E6" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="14" t="s">
-        <v>22</v>
+      <c r="F6" s="19" t="s">
+        <v>108</v>
       </c>
       <c r="G6" s="13" t="s">
         <v>23</v>
@@ -1115,19 +1112,19 @@
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
       <c r="N6" s="13" t="s">
-        <v>37</v>
+        <v>122</v>
       </c>
       <c r="O6" s="13" t="s">
-        <v>38</v>
+        <v>123</v>
       </c>
       <c r="Q6" s="13"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>19</v>
@@ -1139,7 +1136,7 @@
         <v>21</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>22</v>
+        <v>108</v>
       </c>
       <c r="G7" s="13" t="s">
         <v>23</v>
@@ -1153,16 +1150,16 @@
       <c r="N7" s="13"/>
       <c r="O7" s="13"/>
       <c r="P7" s="15" t="s">
-        <v>37</v>
+        <v>122</v>
       </c>
       <c r="Q7" s="13"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>19</v>
@@ -1192,16 +1189,16 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>43</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>45</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>21</v>
@@ -1225,10 +1222,10 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>19</v>
@@ -1240,13 +1237,13 @@
         <v>21</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>48</v>
+        <v>124</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>49</v>
+        <v>125</v>
       </c>
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
@@ -1260,28 +1257,28 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="13" t="s">
         <v>50</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>54</v>
       </c>
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
@@ -1291,16 +1288,14 @@
       <c r="N11" s="13"/>
       <c r="O11" s="13"/>
       <c r="P11" s="15"/>
-      <c r="Q11" s="13" t="s">
-        <v>55</v>
-      </c>
+      <c r="Q11" s="13"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>19</v>
@@ -1345,10 +1340,10 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>19</v>
@@ -1360,7 +1355,7 @@
         <v>21</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G14" s="22" t="s">
         <v>23</v>
@@ -1378,10 +1373,10 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>19</v>
@@ -1393,7 +1388,7 @@
         <v>21</v>
       </c>
       <c r="F15" s="21" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G15" s="22" t="s">
         <v>23</v>
@@ -1411,10 +1406,10 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>19</v>
@@ -1426,7 +1421,7 @@
         <v>21</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G16" s="22" t="s">
         <v>23</v>
@@ -1444,10 +1439,10 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C17" s="13" t="s">
         <v>19</v>
@@ -1459,7 +1454,7 @@
         <v>21</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G17" s="22" t="s">
         <v>23</v>
@@ -1477,10 +1472,10 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>19</v>
@@ -1492,7 +1487,7 @@
         <v>21</v>
       </c>
       <c r="F18" s="21" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G18" s="22" t="s">
         <v>23</v>
@@ -1510,7 +1505,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>
@@ -1531,7 +1526,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
@@ -1552,7 +1547,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
@@ -1573,7 +1568,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
@@ -1594,7 +1589,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
@@ -1615,7 +1610,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
@@ -1636,7 +1631,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
@@ -1657,7 +1652,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
@@ -1678,7 +1673,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B27" s="13"/>
       <c r="C27" s="13"/>
@@ -1707,19 +1702,20 @@
     <hyperlink ref="D11" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="F11" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="D12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="D14" r:id="rId9" xr:uid="{21BE66A9-6327-498E-8C2B-7FE2E11ADD59}"/>
-    <hyperlink ref="F14" r:id="rId10" xr:uid="{12E2B49E-1545-4672-B4A6-DEB308365455}"/>
-    <hyperlink ref="D15" r:id="rId11" xr:uid="{9EBBF634-8706-4A3F-B35D-4E439A536F07}"/>
-    <hyperlink ref="F15" r:id="rId12" xr:uid="{1EAE3C99-A8B6-4606-9E0F-3F30F1A974E1}"/>
-    <hyperlink ref="D16" r:id="rId13" xr:uid="{3BF6D693-1A70-4082-AA38-B89E5A7E3D1E}"/>
-    <hyperlink ref="F16" r:id="rId14" xr:uid="{BB5D3DA6-CFF2-41F1-9364-ACCECDFA487D}"/>
-    <hyperlink ref="D17" r:id="rId15" xr:uid="{E5B91846-B0A7-4689-8939-6B633CD433E1}"/>
-    <hyperlink ref="F17" r:id="rId16" xr:uid="{27A838A4-C4AB-469F-92BD-B56F89856E93}"/>
-    <hyperlink ref="D18" r:id="rId17" xr:uid="{339F8C4E-F6A1-496F-8C6F-34444D3A3D27}"/>
-    <hyperlink ref="F18" r:id="rId18" xr:uid="{B47F81F5-8E63-4013-B98A-3DCC7EF34CE2}"/>
+    <hyperlink ref="D14" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="F14" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D15" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="F15" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="D16" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="F16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="D17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="F17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="D18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="F18" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="F6" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
 
@@ -1767,7 +1763,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>19</v>
@@ -1784,7 +1780,7 @@
         <v>24</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>19</v>
@@ -1801,7 +1797,7 @@
         <v>28</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>19</v>
@@ -1818,7 +1814,7 @@
         <v>33</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>19</v>
@@ -1835,7 +1831,7 @@
         <v>35</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>19</v>
@@ -1849,10 +1845,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>19</v>
@@ -1866,10 +1862,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>19</v>
@@ -1883,10 +1879,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>19</v>
@@ -1900,10 +1896,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>19</v>
@@ -1917,10 +1913,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>19</v>
@@ -1934,10 +1930,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>19</v>
@@ -1951,10 +1947,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>19</v>
@@ -1968,10 +1964,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>19</v>
@@ -1985,10 +1981,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>19</v>
@@ -2002,10 +1998,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>19</v>
@@ -2019,10 +2015,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C17" s="13" t="s">
         <v>19</v>
@@ -2036,10 +2032,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D16" r:id="rId1" display="https://qat01.frontier.com/" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="D17" r:id="rId2" display="https://qat01.frontier.com/" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="D3" r:id="rId3" xr:uid="{2243F20E-836A-44C8-A7E8-FEF69ED0BABA}"/>
-    <hyperlink ref="D2" r:id="rId4" xr:uid="{4A26EF29-4866-422F-8BC1-B340F7348B64}"/>
+    <hyperlink ref="D16" r:id="rId1" display="https://qat01.frontier.com/" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D17" r:id="rId2" display="https://qat01.frontier.com/" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="D2" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -2097,16 +2093,16 @@
         <v>6</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="J1" s="17" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K1" s="17" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2114,7 +2110,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>19</v>
@@ -2128,16 +2124,16 @@
       <c r="F2" s="7"/>
       <c r="G2" s="5"/>
       <c r="H2" s="6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -2145,7 +2141,7 @@
         <v>24</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>19</v>
@@ -2168,7 +2164,7 @@
         <v>28</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>19</v>
@@ -2195,7 +2191,7 @@
         <v>33</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>19</v>
@@ -2218,7 +2214,7 @@
         <v>35</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>19</v>
@@ -2238,10 +2234,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>19</v>
@@ -2261,10 +2257,10 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>19</v>
@@ -2284,10 +2280,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>19</v>
@@ -2307,10 +2303,10 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>19</v>
@@ -2348,16 +2344,16 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1:E1048576"/>
+      <selection pane="bottomRight" activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" style="11" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" style="11" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" style="11" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" style="11" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="6.7109375" style="11" customWidth="1"/>
     <col min="8" max="16384" width="6.7109375" style="11"/>
   </cols>
@@ -2384,7 +2380,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>19</v>
@@ -2401,7 +2397,7 @@
         <v>24</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>19</v>
@@ -2418,7 +2414,7 @@
         <v>28</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>19</v>
@@ -2435,7 +2431,7 @@
         <v>33</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>19</v>
@@ -2452,7 +2448,7 @@
         <v>35</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>19</v>
@@ -2466,10 +2462,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>19</v>
@@ -2483,10 +2479,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>19</v>
@@ -2500,10 +2496,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>19</v>
@@ -2517,10 +2513,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>19</v>
@@ -2534,10 +2530,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>19</v>
@@ -2551,10 +2547,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>19</v>
@@ -2568,10 +2564,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>19</v>
@@ -2585,10 +2581,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>19</v>
@@ -2602,10 +2598,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>19</v>
@@ -2619,10 +2615,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>19</v>
@@ -2636,10 +2632,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C17" s="13" t="s">
         <v>19</v>

</xml_diff>